<commit_message>
Primera y corregida versión de inicio
</commit_message>
<xml_diff>
--- a/MazdaMX2/Dealers.xlsx
+++ b/MazdaMX2/Dealers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\Mvelasco-git\MazdaMX2\MazdaMX2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\MazdaMX2\MazdaMX2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879F40D1-E904-4A25-B1D9-70EB545B4C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D63F5D0-0059-4707-8E89-8DF29D2E3515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="121">
   <si>
     <t>VERIFICAR</t>
   </si>
@@ -253,21 +253,12 @@
     <t>mazda3-sedan-flydown-perfil-v1</t>
   </si>
   <si>
-    <t>mazda3-hatchback-2024-flydown-v2</t>
-  </si>
-  <si>
     <t>cx-3-flydown-perfil-v1</t>
   </si>
   <si>
-    <t>cx-30-flydown-perfil-v1</t>
-  </si>
-  <si>
     <t>cx-5-flydown-perfil-v1</t>
   </si>
   <si>
-    <t>cx-50-2024-flydown-v1</t>
-  </si>
-  <si>
     <t>cx-90-2024-flydown-v1</t>
   </si>
   <si>
@@ -310,12 +301,6 @@
     <t>542,900</t>
   </si>
   <si>
-    <t>448,900</t>
-  </si>
-  <si>
-    <t>488,900</t>
-  </si>
-  <si>
     <t>558,900</t>
   </si>
   <si>
@@ -328,27 +313,15 @@
     <t>450,900</t>
   </si>
   <si>
-    <t>459,900</t>
-  </si>
-  <si>
     <t>495,900</t>
   </si>
   <si>
-    <t>505,900</t>
-  </si>
-  <si>
-    <t>545,900</t>
-  </si>
-  <si>
     <t>618,900</t>
   </si>
   <si>
     <t>688,900</t>
   </si>
   <si>
-    <t>805,900</t>
-  </si>
-  <si>
     <t>Signature MHEV</t>
   </si>
   <si>
@@ -365,6 +338,51 @@
   </si>
   <si>
     <t>619,900</t>
+  </si>
+  <si>
+    <t>mazda-cx-70-lateral-inclinado-v2</t>
+  </si>
+  <si>
+    <t>MAZDA CX-70</t>
+  </si>
+  <si>
+    <t>mazda3-hatchback-flydown-inclinado-v1</t>
+  </si>
+  <si>
+    <t>1,038,000</t>
+  </si>
+  <si>
+    <t>280</t>
+  </si>
+  <si>
+    <t>332</t>
+  </si>
+  <si>
+    <t>453,900</t>
+  </si>
+  <si>
+    <t>563,900</t>
+  </si>
+  <si>
+    <t>815,900</t>
+  </si>
+  <si>
+    <t>436,900</t>
+  </si>
+  <si>
+    <t>466,900</t>
+  </si>
+  <si>
+    <t>512,900</t>
+  </si>
+  <si>
+    <t>552,900</t>
+  </si>
+  <si>
+    <t>mazda-cx-30-flydown-perfil-v2</t>
+  </si>
+  <si>
+    <t>mazda-cx-50-flydown-v2</t>
   </si>
 </sst>
 </file>
@@ -687,34 +705,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ12"/>
+  <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="3" width="16.09765625" customWidth="1"/>
-    <col min="4" max="4" width="12.09765625" customWidth="1"/>
-    <col min="5" max="5" width="10.796875" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.125" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="10.75" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="13.296875" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="9" width="4" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.69921875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.296875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.296875" customWidth="1"/>
+    <col min="10" max="10" width="8.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.25" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
-    <col min="14" max="15" width="8.796875" style="1"/>
-    <col min="16" max="16" width="9.296875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.69921875" customWidth="1"/>
+    <col min="14" max="15" width="8.75" style="1"/>
+    <col min="16" max="16" width="9.25" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.75" customWidth="1"/>
     <col min="18" max="18" width="9" style="1"/>
-    <col min="19" max="21" width="8.796875" style="1"/>
-    <col min="22" max="22" width="13.8984375" customWidth="1"/>
-    <col min="25" max="25" width="8.69921875" customWidth="1"/>
-    <col min="27" max="27" width="10.09765625" customWidth="1"/>
-    <col min="32" max="32" width="13.8984375" customWidth="1"/>
+    <col min="19" max="21" width="8.75" style="1"/>
+    <col min="22" max="22" width="13.875" customWidth="1"/>
+    <col min="25" max="25" width="8.75" customWidth="1"/>
+    <col min="27" max="27" width="10.125" customWidth="1"/>
+    <col min="32" max="32" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -850,7 +870,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>38</v>
@@ -865,7 +885,7 @@
         <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>38</v>
@@ -880,7 +900,7 @@
         <v>42</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>38</v>
@@ -895,13 +915,13 @@
         <v>52</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>50</v>
@@ -930,7 +950,7 @@
         <v>41</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>38</v>
@@ -942,10 +962,10 @@
         <v>40</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>38</v>
@@ -960,13 +980,13 @@
         <v>52</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>50</v>
@@ -998,7 +1018,7 @@
         <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>45</v>
@@ -1013,7 +1033,7 @@
         <v>41</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>45</v>
@@ -1028,7 +1048,7 @@
         <v>47</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>48</v>
@@ -1043,7 +1063,7 @@
         <v>51</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>45</v>
@@ -1058,7 +1078,7 @@
         <v>52</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AC4" s="1" t="s">
         <v>53</v>
@@ -1078,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>68</v>
@@ -1090,13 +1110,13 @@
         <v>43</v>
       </c>
       <c r="F5">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G5" t="s">
         <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>45</v>
@@ -1126,7 +1146,7 @@
         <v>52</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>53</v>
@@ -1148,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>69</v>
@@ -1166,7 +1186,7 @@
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>49</v>
@@ -1181,7 +1201,7 @@
         <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>49</v>
@@ -1196,7 +1216,7 @@
         <v>51</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>49</v>
@@ -1213,10 +1233,10 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>69</v>
@@ -1228,13 +1248,13 @@
         <v>56</v>
       </c>
       <c r="F7">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>45</v>
@@ -1246,25 +1266,25 @@
         <v>46</v>
       </c>
       <c r="L7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>51</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>45</v>
@@ -1279,7 +1299,7 @@
         <v>52</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>53</v>
@@ -1296,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>69</v>
@@ -1314,7 +1334,7 @@
         <v>41</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>61</v>
@@ -1329,7 +1349,7 @@
         <v>62</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>61</v>
@@ -1344,7 +1364,7 @@
         <v>52</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>63</v>
@@ -1362,10 +1382,10 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>69</v>
@@ -1377,13 +1397,13 @@
         <v>56</v>
       </c>
       <c r="F9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>63</v>
@@ -1400,48 +1420,48 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
       </c>
       <c r="F10">
-        <v>2024</v>
-      </c>
-      <c r="G10" s="2" t="s">
+        <v>2025</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="E11" t="s">
         <v>56</v>
@@ -1449,34 +1469,34 @@
       <c r="F11">
         <v>2024</v>
       </c>
-      <c r="G11" t="s">
-        <v>41</v>
+      <c r="G11" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>50</v>
+        <v>101</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:36">
       <c r="A12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
         <v>56</v>
@@ -1485,10 +1505,10 @@
         <v>2024</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>65</v>
@@ -1497,6 +1517,41 @@
         <v>66</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="A13" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>2024</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se sube cambios importantes en codigo para su buen funcionamiento
</commit_message>
<xml_diff>
--- a/MazdaMX2/Dealers.xlsx
+++ b/MazdaMX2/Dealers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\MazdaMX2\MazdaMX2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D63F5D0-0059-4707-8E89-8DF29D2E3515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5666B-0994-4285-B2BB-574B777AD08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="116">
   <si>
     <t>VERIFICAR</t>
   </si>
@@ -163,12 +163,6 @@
     <t>2.5L</t>
   </si>
   <si>
-    <t>i Sport MHEV</t>
-  </si>
-  <si>
-    <t>153</t>
-  </si>
-  <si>
     <t>148</t>
   </si>
   <si>
@@ -208,9 +202,6 @@
     <t>188</t>
   </si>
   <si>
-    <t>s Grand Touring</t>
-  </si>
-  <si>
     <t>228</t>
   </si>
   <si>
@@ -244,90 +235,27 @@
     <t>CATEGORIA</t>
   </si>
   <si>
-    <t>mazda2-sedan-flydown-v2-rojo</t>
-  </si>
-  <si>
-    <t>mazda2-hatchback-signature-rojo</t>
-  </si>
-  <si>
-    <t>mazda3-sedan-flydown-perfil-v1</t>
-  </si>
-  <si>
-    <t>cx-3-flydown-perfil-v1</t>
-  </si>
-  <si>
     <t>cx-5-flydown-perfil-v1</t>
   </si>
   <si>
-    <t>cx-90-2024-flydown-v1</t>
-  </si>
-  <si>
     <t>mx-5-carro-rojo-deportivo</t>
   </si>
   <si>
     <t>carro-mazda-mx-5-gris-v1</t>
   </si>
   <si>
-    <t>288,900</t>
-  </si>
-  <si>
-    <t>318,900</t>
-  </si>
-  <si>
-    <t>358,900</t>
-  </si>
-  <si>
-    <t>388,900</t>
-  </si>
-  <si>
     <t>141</t>
   </si>
   <si>
     <t>137</t>
   </si>
   <si>
-    <t>392,900</t>
-  </si>
-  <si>
-    <t>422,900</t>
-  </si>
-  <si>
-    <t>462,900</t>
-  </si>
-  <si>
-    <t>472,900</t>
-  </si>
-  <si>
-    <t>542,900</t>
-  </si>
-  <si>
-    <t>558,900</t>
-  </si>
-  <si>
-    <t>380,900</t>
-  </si>
-  <si>
-    <t>410,900</t>
-  </si>
-  <si>
-    <t>450,900</t>
-  </si>
-  <si>
     <t>495,900</t>
   </si>
   <si>
-    <t>618,900</t>
-  </si>
-  <si>
-    <t>688,900</t>
-  </si>
-  <si>
     <t>Signature MHEV</t>
   </si>
   <si>
-    <t>1,138,000</t>
-  </si>
-  <si>
     <t>340</t>
   </si>
   <si>
@@ -349,9 +277,6 @@
     <t>mazda3-hatchback-flydown-inclinado-v1</t>
   </si>
   <si>
-    <t>1,038,000</t>
-  </si>
-  <si>
     <t>280</t>
   </si>
   <si>
@@ -383,6 +308,66 @@
   </si>
   <si>
     <t>mazda-cx-50-flydown-v2</t>
+  </si>
+  <si>
+    <t>295,900</t>
+  </si>
+  <si>
+    <t>325,900</t>
+  </si>
+  <si>
+    <t>365,900</t>
+  </si>
+  <si>
+    <t>395,900</t>
+  </si>
+  <si>
+    <t>386,900</t>
+  </si>
+  <si>
+    <t>416,900</t>
+  </si>
+  <si>
+    <t>mazda-mazda2-sedan-rojo-perfil-v1</t>
+  </si>
+  <si>
+    <t>automovil-mazda2-hatchback-rojo-costado</t>
+  </si>
+  <si>
+    <t>mazda-mexico-cx-3-flydown-perfil-v1</t>
+  </si>
+  <si>
+    <t>548,900</t>
+  </si>
+  <si>
+    <t>608,900</t>
+  </si>
+  <si>
+    <t>678,900</t>
+  </si>
+  <si>
+    <t>mazda3-sedan-flydown-perfil-v2</t>
+  </si>
+  <si>
+    <t>397,900</t>
+  </si>
+  <si>
+    <t>437,900</t>
+  </si>
+  <si>
+    <t>477,900</t>
+  </si>
+  <si>
+    <t>547,900</t>
+  </si>
+  <si>
+    <t>958,000</t>
+  </si>
+  <si>
+    <t>mazda-cx-90-flydown-rojo-artesano-inclinado-v1.png</t>
+  </si>
+  <si>
+    <t>1,058,000</t>
   </si>
 </sst>
 </file>
@@ -707,15 +692,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="11.75" customWidth="1"/>
     <col min="4" max="4" width="12.125" customWidth="1"/>
     <col min="5" max="5" width="10.75" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
@@ -745,7 +730,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -852,10 +837,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
@@ -864,13 +849,13 @@
         <v>36</v>
       </c>
       <c r="F2">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G2" t="s">
         <v>37</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>38</v>
@@ -885,7 +870,7 @@
         <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>38</v>
@@ -897,10 +882,10 @@
         <v>40</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>38</v>
@@ -912,19 +897,19 @@
         <v>40</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -932,10 +917,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
@@ -944,13 +929,13 @@
         <v>43</v>
       </c>
       <c r="F3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G3" t="s">
         <v>41</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>38</v>
@@ -962,10 +947,10 @@
         <v>40</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>38</v>
@@ -977,19 +962,19 @@
         <v>40</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -1000,10 +985,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
         <v>44</v>
@@ -1012,13 +997,13 @@
         <v>36</v>
       </c>
       <c r="F4">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G4" t="s">
         <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>45</v>
@@ -1033,7 +1018,7 @@
         <v>41</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>45</v>
@@ -1045,50 +1030,38 @@
         <v>46</v>
       </c>
       <c r="Q4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="U4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" t="s">
         <v>50</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="W4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="Y4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z4" t="s">
         <v>46</v>
       </c>
-      <c r="AA4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>46</v>
-      </c>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
@@ -1098,10 +1071,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>
@@ -1116,7 +1089,7 @@
         <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>45</v>
@@ -1128,10 +1101,10 @@
         <v>46</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>45</v>
@@ -1143,16 +1116,16 @@
         <v>46</v>
       </c>
       <c r="Q5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>46</v>
@@ -1168,84 +1141,70 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G6" t="s">
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
         <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>51</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="R6" s="3"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:36">
       <c r="A7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7">
         <v>2025</v>
@@ -1254,7 +1213,7 @@
         <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>45</v>
@@ -1269,7 +1228,7 @@
         <v>41</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>45</v>
@@ -1281,10 +1240,10 @@
         <v>46</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>45</v>
@@ -1296,16 +1255,16 @@
         <v>46</v>
       </c>
       <c r="V7" t="s">
+        <v>50</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y7" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="Z7" s="1" t="s">
         <v>46</v>
@@ -1316,28 +1275,28 @@
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G8" t="s">
         <v>41</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>45</v>
@@ -1346,13 +1305,13 @@
         <v>46</v>
       </c>
       <c r="L8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>45</v>
@@ -1361,16 +1320,16 @@
         <v>46</v>
       </c>
       <c r="Q8" t="s">
+        <v>50</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T8" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>46</v>
@@ -1382,34 +1341,34 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9">
         <v>2025</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>46</v>
@@ -1420,16 +1379,16 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10">
         <v>2025</v>
@@ -1438,51 +1397,51 @@
         <v>42</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>2025</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11">
-        <v>2024</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="K11" s="3" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:36">
@@ -1490,16 +1449,16 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12">
         <v>2024</v>
@@ -1508,16 +1467,16 @@
         <v>41</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:36">
@@ -1525,34 +1484,34 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F13">
         <v>2024</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se depura codigo de automatización y subimos codigo mejorado 04042025
</commit_message>
<xml_diff>
--- a/MazdaMX2/Dealers.xlsx
+++ b/MazdaMX2/Dealers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\MazdaMX2\MazdaMX2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5666B-0994-4285-B2BB-574B777AD08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC1A355-7D33-43BA-8E28-781C6A5CFE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
   <si>
     <t>VERIFICAR</t>
   </si>
@@ -193,9 +193,6 @@
     <t>MAZDA CX-30</t>
   </si>
   <si>
-    <t>519,900</t>
-  </si>
-  <si>
     <t>MAZDA CX-5</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>cx-5-flydown-perfil-v1</t>
   </si>
   <si>
-    <t>mx-5-carro-rojo-deportivo</t>
-  </si>
-  <si>
     <t>carro-mazda-mx-5-gris-v1</t>
   </si>
   <si>
@@ -265,9 +259,6 @@
     <t>3.3L</t>
   </si>
   <si>
-    <t>619,900</t>
-  </si>
-  <si>
     <t>mazda-cx-70-lateral-inclinado-v2</t>
   </si>
   <si>
@@ -310,18 +301,6 @@
     <t>mazda-cx-50-flydown-v2</t>
   </si>
   <si>
-    <t>295,900</t>
-  </si>
-  <si>
-    <t>325,900</t>
-  </si>
-  <si>
-    <t>365,900</t>
-  </si>
-  <si>
-    <t>395,900</t>
-  </si>
-  <si>
     <t>386,900</t>
   </si>
   <si>
@@ -368,6 +347,54 @@
   </si>
   <si>
     <t>1,058,000</t>
+  </si>
+  <si>
+    <t>300,900</t>
+  </si>
+  <si>
+    <t>330,900</t>
+  </si>
+  <si>
+    <t>370,900</t>
+  </si>
+  <si>
+    <t>398,900</t>
+  </si>
+  <si>
+    <t>mazda-mx-5-35-aniversario-flydown-perspectiva-v1</t>
+  </si>
+  <si>
+    <t>MAZDA MX-5 35° ANIVERSARIO</t>
+  </si>
+  <si>
+    <t>639,900</t>
+  </si>
+  <si>
+    <t>35° Aniversario</t>
+  </si>
+  <si>
+    <t>mx-5-carro-rojo-deportivo-inclinado-v1-1</t>
+  </si>
+  <si>
+    <t>529,900</t>
+  </si>
+  <si>
+    <t>629,900</t>
+  </si>
+  <si>
+    <t>PICKUPS</t>
+  </si>
+  <si>
+    <t>MAZDA BT-50</t>
+  </si>
+  <si>
+    <t>829,900</t>
+  </si>
+  <si>
+    <t>3.0L</t>
+  </si>
+  <si>
+    <t>mazda-bt-50-roja-flydown-inclinado-v2</t>
   </si>
 </sst>
 </file>
@@ -690,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ13"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
@@ -730,7 +757,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -834,13 +861,13 @@
     </row>
     <row r="2" spans="1:36">
       <c r="A2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
@@ -855,7 +882,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>38</v>
@@ -870,7 +897,7 @@
         <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>38</v>
@@ -885,7 +912,7 @@
         <v>49</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>38</v>
@@ -900,13 +927,13 @@
         <v>50</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>48</v>
@@ -914,13 +941,13 @@
     </row>
     <row r="3" spans="1:36">
       <c r="A3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
@@ -935,7 +962,7 @@
         <v>41</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>38</v>
@@ -950,7 +977,7 @@
         <v>49</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>38</v>
@@ -965,13 +992,13 @@
         <v>50</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>48</v>
@@ -985,10 +1012,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
         <v>44</v>
@@ -1003,7 +1030,7 @@
         <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>45</v>
@@ -1018,7 +1045,7 @@
         <v>41</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>45</v>
@@ -1033,7 +1060,7 @@
         <v>49</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>45</v>
@@ -1048,7 +1075,7 @@
         <v>50</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>51</v>
@@ -1071,10 +1098,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>
@@ -1089,7 +1116,7 @@
         <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>45</v>
@@ -1104,7 +1131,7 @@
         <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>45</v>
@@ -1119,7 +1146,7 @@
         <v>50</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>51</v>
@@ -1141,10 +1168,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
         <v>53</v>
@@ -1159,7 +1186,7 @@
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>47</v>
@@ -1174,7 +1201,7 @@
         <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>47</v>
@@ -1195,10 +1222,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
         <v>56</v>
@@ -1213,7 +1240,7 @@
         <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>45</v>
@@ -1228,7 +1255,7 @@
         <v>41</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>45</v>
@@ -1243,7 +1270,7 @@
         <v>49</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>45</v>
@@ -1258,7 +1285,7 @@
         <v>50</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>51</v>
@@ -1275,13 +1302,13 @@
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -1293,10 +1320,10 @@
         <v>41</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>45</v>
@@ -1308,10 +1335,10 @@
         <v>49</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>45</v>
@@ -1323,7 +1350,7 @@
         <v>50</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>51</v>
@@ -1344,13 +1371,13 @@
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
@@ -1362,10 +1389,10 @@
         <v>50</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>52</v>
@@ -1379,13 +1406,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -1397,30 +1424,30 @@
         <v>42</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
@@ -1429,19 +1456,19 @@
         <v>2025</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:36">
@@ -1449,34 +1476,34 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="s">
-        <v>61</v>
+        <v>120</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
       </c>
       <c r="F12">
-        <v>2024</v>
-      </c>
-      <c r="G12" t="s">
-        <v>41</v>
+        <v>2025</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>48</v>
+        <v>122</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:36">
@@ -1484,38 +1511,108 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>54</v>
       </c>
       <c r="F13">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14">
+        <v>2025</v>
+      </c>
+      <c r="G14" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="H14" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="K14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36">
+      <c r="A15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <v>2025</v>
+      </c>
+      <c r="G15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>